<commit_message>
Enabled - background automation Now the Survey Robot will not interact with persons computer at any time
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srdjan.suc\Downloads\SurveyRobot.connect.20200228\SurveyRobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CF394F-6EDB-41D6-974C-CF4C14759603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4306B17-2BD2-4F03-9A3B-38FDE49DA4C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4356" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4704" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="4-13" sheetId="7" r:id="rId1"/>
-    <sheet name="Sum" sheetId="1" r:id="rId2"/>
+    <sheet name="Sum" sheetId="1" r:id="rId1"/>
+    <sheet name="4-13" sheetId="7" r:id="rId2"/>
     <sheet name="Source" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,28 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
-  <si>
-    <t>Work from home</t>
-  </si>
-  <si>
-    <t>Work from office</t>
-  </si>
-  <si>
-    <t>Customer site</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>number of respondant</t>
-  </si>
-  <si>
-    <t>number of nonrespondant</t>
-  </si>
-  <si>
-    <t>Work arrangement</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>count</t>
   </si>
@@ -64,16 +43,37 @@
     <t>Date</t>
   </si>
   <si>
-    <t>total</t>
+    <t>Raspored rada</t>
   </si>
   <si>
-    <t>num of participant</t>
+    <t>procenat učešća</t>
   </si>
   <si>
-    <t>participat ratio</t>
+    <t>povišene temperature</t>
   </si>
   <si>
-    <t>abnormal body temperture</t>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Rad od kuće</t>
+  </si>
+  <si>
+    <t>Rad kod korisnika</t>
+  </si>
+  <si>
+    <t>Rad iz kancelarije</t>
+  </si>
+  <si>
+    <t>ukupan broj ispitanika</t>
+  </si>
+  <si>
+    <t>broj ispitanika koji nisu popunili obrazac</t>
+  </si>
+  <si>
+    <t>Ukupan broj ispitanika</t>
+  </si>
+  <si>
+    <t>Broj popunjenih obrazaca</t>
   </si>
   <si>
     <t>ID</t>
@@ -91,52 +91,34 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Your name</t>
+    <t>Email adresa</t>
   </si>
   <si>
-    <t>Your Email</t>
+    <t>Lokacija kancelarije Ibis Instruments-a</t>
   </si>
   <si>
-    <t>Ibis Instruments office location</t>
+    <t>Imate li respiratorne simptome (kašalj, nedostatak daha, curenje nosa, grlobolja)?</t>
   </si>
   <si>
-    <t>Do you have any respiratory symptoms (cough, shortness of breath, runny nose, sore throat)?</t>
+    <t>Da li ste bili u kontaktu sa nekim osobama koje su potvrđene da boluju od Covid-19?</t>
   </si>
   <si>
-    <t>Have you been in contact with any persons confirmed with Covid-19?</t>
+    <t>Molimo vas da unesete vašu trenutnu temperaturu</t>
   </si>
   <si>
-    <t>Have you visited any highly infected areas (such as Italy or Spain) in the past 14 days?</t>
-  </si>
-  <si>
-    <t>Please enter your temperature recorded</t>
-  </si>
-  <si>
-    <t>How do you feel?</t>
+    <t>Kako se osećate?</t>
   </si>
   <si>
     <t>anonymous</t>
   </si>
   <si>
-    <t>Srdjan Suc</t>
-  </si>
-  <si>
     <t>srdjan.suc@hotmail.com</t>
   </si>
   <si>
-    <t>Belgrade</t>
+    <t>Beograd</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>Marko Zvale</t>
-  </si>
-  <si>
-    <t>sucdotaacc1@gmail.com</t>
+    <t>Ne</t>
   </si>
 </sst>
 </file>
@@ -347,6 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,7 +357,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,8 +409,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>work arrangement</a:t>
+              <a:rPr lang="sr-Latn-RS" altLang="zh-CN"/>
+              <a:t>Raspored</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sr-Latn-RS" altLang="zh-CN" baseline="0"/>
+              <a:t> rada</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN" altLang="en-US"/>
           </a:p>
@@ -706,16 +692,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Work from home</c:v>
+                  <c:v>Rad od kuće</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Customer site</c:v>
+                  <c:v>Rad kod korisnika</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Work from office</c:v>
+                  <c:v>Rad iz kancelarije</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Others</c:v>
+                  <c:v>Other</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -727,7 +713,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -873,8 +859,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>last 7 days work arrangement statistics</a:t>
+              <a:rPr lang="sr-Latn-RS" altLang="zh-CN"/>
+              <a:t>Statistika o rasporedu</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sr-Latn-RS" altLang="zh-CN" baseline="0"/>
+              <a:t> rada u poslednjih 7 dana</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -961,7 +951,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Work from home</c:v>
+                  <c:v>Rad od kuće</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1056,20 +1046,23 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Source!$D$2:$D$8</c:f>
+              <c:f>Source!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43932</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43932</c:v>
+                  <c:v>43933</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>43934</c:v>
                 </c:pt>
               </c:numCache>
@@ -1077,21 +1070,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Source!$E$2:$E$8</c:f>
+              <c:f>Source!$E$2:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1111,7 +1107,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Customer site</c:v>
+                  <c:v>Rad kod korisnika</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1206,20 +1202,23 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Source!$D$2:$D$8</c:f>
+              <c:f>Source!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43932</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43932</c:v>
+                  <c:v>43933</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>43934</c:v>
                 </c:pt>
               </c:numCache>
@@ -1227,20 +1226,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Source!$F$2:$F$8</c:f>
+              <c:f>Source!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1261,7 +1263,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Work from office</c:v>
+                  <c:v>Rad iz kancelarije</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1356,20 +1358,23 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Source!$D$2:$D$8</c:f>
+              <c:f>Source!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43932</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43932</c:v>
+                  <c:v>43933</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>43934</c:v>
                 </c:pt>
               </c:numCache>
@@ -1377,20 +1382,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Source!$G$2:$G$8</c:f>
+              <c:f>Source!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1411,7 +1419,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Others</c:v>
+                  <c:v>Other</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1506,20 +1514,23 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Source!$D$2:$D$8</c:f>
+              <c:f>Source!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43932</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43932</c:v>
+                  <c:v>43933</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>43934</c:v>
                 </c:pt>
               </c:numCache>
@@ -1527,20 +1538,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Source!$H$2:$H$8</c:f>
+              <c:f>Source!$H$2:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1757,9 +1771,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr" rtl="0">
-              <a:defRPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="sr-Latn-RS" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="44546A"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1767,23 +1784,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="44546A"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+              <a:rPr lang="sr-Latn-RS" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
               </a:rPr>
-              <a:t>last 7 days participation statistics</a:t>
+              <a:t>Statistika učešća u poslednjih 7 dana</a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="44546A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
             </a:endParaRPr>
           </a:p>
         </c:rich>
@@ -1801,9 +1808,12 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
-            <a:defRPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr lang="sr-Latn-RS" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="44546A"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1869,7 +1879,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>number of respondant</c:v>
+                  <c:v>ukupan broj ispitanika</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1887,20 +1897,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Source!$D$2:$D$8</c:f>
+              <c:f>Source!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43932</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43932</c:v>
+                  <c:v>43933</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>43934</c:v>
                 </c:pt>
               </c:numCache>
@@ -1908,21 +1921,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Source!$I$2:$I$8</c:f>
+              <c:f>Source!$I$2:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1942,7 +1958,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>number of nonrespondant</c:v>
+                  <c:v>broj ispitanika koji nisu popunili obrazac</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1960,20 +1976,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Source!$D$2:$D$8</c:f>
+              <c:f>Source!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43932</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43932</c:v>
+                  <c:v>43933</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>43934</c:v>
                 </c:pt>
               </c:numCache>
@@ -1981,21 +2000,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Source!$J$2:$J$8</c:f>
+              <c:f>Source!$J$2:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2043,7 +2065,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="sr-Latn-RS" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2101,7 +2123,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="sr-Latn-RS" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2143,7 +2165,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="sr-Latn-RS" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2187,7 +2209,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr lang="sr-Latn-RS"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -4194,150 +4216,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E608AEBF-5D2F-474E-9451-BDE743E90208}">
-  <dimension ref="A1:N3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>17</v>
-      </c>
-      <c r="B2" s="22">
-        <v>43934.432210648149</v>
-      </c>
-      <c r="C2" s="22">
-        <v>43934.43240740741</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>18</v>
-      </c>
-      <c r="B3" s="22">
-        <v>43934.449016203704</v>
-      </c>
-      <c r="C3" s="22">
-        <v>43934.449282407404</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3">
-        <v>36</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4353,19 +4236,19 @@
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="2:15" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="13" t="str">
-        <f ca="1">TEXT(TODAY(),"yyyy/MM/dd")&amp;" health screening statistics"</f>
-        <v>2020/04/13 health screening statistics</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="15"/>
+      <c r="B2" s="14" t="str">
+        <f ca="1">TEXT(TODAY(),"yyyy/MM/dd")&amp;" Statistika zdravstvenog ispitivanja"</f>
+        <v>2020/04/13 Statistika zdravstvenog ispitivanja</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
@@ -4404,11 +4287,11 @@
       <c r="K5" s="9"/>
     </row>
     <row r="6" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -4418,11 +4301,11 @@
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="20">
+      <c r="B7" s="21">
         <v>2</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -4434,11 +4317,11 @@
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="B8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -4448,11 +4331,11 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="20">
-        <v>2</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>1</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -4462,11 +4345,11 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -4478,12 +4361,12 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="16">
+      <c r="B11" s="17">
         <f>B9/B7</f>
-        <v>1</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -4493,11 +4376,11 @@
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -4507,11 +4390,11 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="20">
+      <c r="B13" s="21">
         <v>0</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -4934,12 +4817,98 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB84E58-8B36-41FC-B1E8-95F856878F97}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2" s="13">
+        <v>43934.620671296296</v>
+      </c>
+      <c r="C2" s="13">
+        <v>43934.620844907404</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2">
+        <v>36</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D753C98C-D5A1-4783-A426-AB38939B5182}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4957,72 +4926,132 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43930</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1"/>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="D3" s="3">
+        <v>43931</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="D4" s="3">
+        <v>43932</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>43931</v>
+        <v>43933</v>
       </c>
       <c r="E5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -5041,34 +5070,14 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D6" s="3">
-        <v>43932</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D7" s="3">
-        <v>43933</v>
+        <v>43934</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -5080,10 +5089,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -5091,7 +5100,7 @@
         <v>43934</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -5102,12 +5111,12 @@
       <c r="H8" s="1">
         <v>0</v>
       </c>
-      <c r="I8" s="1">
-        <v>2</v>
+      <c r="I8">
+        <v>1</v>
       </c>
       <c r="J8">
-        <f>2-2</f>
-        <v>0</v>
+        <f>2-1</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>